<commit_message>
Added module 2 discussion
</commit_message>
<xml_diff>
--- a/Module2/Assignment/Worksheet 2 - Immune Cell Type.xlsx
+++ b/Module2/Assignment/Worksheet 2 - Immune Cell Type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvesgreatti/github/Immunoengineering/Module2/Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{786D58DD-296C-4048-82AC-7A32253D68F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBF13D3-E0AB-E44D-8A86-62C2C63EE556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29240" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cell summary sheet blank" sheetId="4" r:id="rId1"/>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>How</t>
-  </si>
-  <si>
-    <t>Nuetrophils</t>
   </si>
   <si>
     <t>Dendritic Cells</t>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>5. If you do not want to fill in the excel sheet, please write each major category with functions in bullet point below.</t>
+  </si>
+  <si>
+    <t>Neutrophils</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -433,7 +433,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -449,7 +449,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -459,22 +459,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1332,86 +1332,86 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="150" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.125" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="20.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="20.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="15.625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="20.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="20.6640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="23" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.625" customWidth="1"/>
-    <col min="13" max="14" width="20.625" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="14" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="35" x14ac:dyDescent="1.4">
+    <row r="1" spans="1:14" ht="35" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="23" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="23" x14ac:dyDescent="1">
-      <c r="A3" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="23" x14ac:dyDescent="1">
+    <row r="4" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="23" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="22.75" x14ac:dyDescent="0.95">
-      <c r="A5" s="29" t="s">
+    <row r="6" spans="1:14" ht="23" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="22.75" x14ac:dyDescent="0.95">
-      <c r="A6" s="29" t="s">
+    <row r="7" spans="1:14" ht="23" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="22.75" x14ac:dyDescent="0.95">
-      <c r="A7" s="29" t="s">
+    <row r="8" spans="1:14" ht="23" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="22.75" x14ac:dyDescent="0.95">
-      <c r="A8" s="29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="30.25" x14ac:dyDescent="1">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:14" ht="32" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
       <c r="I11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
       <c r="N11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.8"/>
-    <row r="13" spans="1:14" s="6" customFormat="1" ht="39.25" thickBot="1" x14ac:dyDescent="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:14" s="6" customFormat="1" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
@@ -1449,33 +1449,33 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A14" s="31" t="s">
-        <v>29</v>
+    <row r="14" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="35" t="s">
+        <v>28</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="12"/>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="35" t="s">
         <v>7</v>
       </c>
       <c r="G14" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H14" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="35" t="s">
         <v>22</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="K14" s="31" t="s">
-        <v>23</v>
       </c>
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
       <c r="N14" s="12"/>
     </row>
-    <row r="15" spans="1:14" ht="71.5" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:14" ht="71.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="32"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1491,7 +1491,7 @@
       <c r="M15" s="20"/>
       <c r="N15" s="14"/>
     </row>
-    <row r="16" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="32"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -1500,20 +1500,20 @@
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
       <c r="I16" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K16" s="32"/>
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="14"/>
     </row>
-    <row r="17" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="32"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
       <c r="D17" s="14"/>
       <c r="F17" s="32" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -1523,7 +1523,7 @@
       <c r="M17" s="20"/>
       <c r="N17" s="14"/>
     </row>
-    <row r="18" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="32"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -1537,7 +1537,7 @@
       <c r="M18" s="20"/>
       <c r="N18" s="14"/>
     </row>
-    <row r="19" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="32"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -1551,27 +1551,27 @@
       <c r="M19" s="21"/>
       <c r="N19" s="14"/>
     </row>
-    <row r="20" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="33"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="14"/>
-      <c r="F20" s="34" t="s">
-        <v>12</v>
+      <c r="F20" s="30" t="s">
+        <v>11</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
       <c r="I20" s="14"/>
-      <c r="K20" s="34" t="s">
+      <c r="K20" s="30" t="s">
         <v>6</v>
       </c>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
       <c r="N20" s="14"/>
     </row>
-    <row r="21" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A21" s="34" t="s">
-        <v>19</v>
+    <row r="21" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="30" t="s">
+        <v>18</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -1585,7 +1585,7 @@
       <c r="M21" s="20"/>
       <c r="N21" s="14"/>
     </row>
-    <row r="22" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="32"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -1599,7 +1599,7 @@
       <c r="M22" s="20"/>
       <c r="N22" s="14"/>
     </row>
-    <row r="23" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="32"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -1613,7 +1613,7 @@
       <c r="M23" s="20"/>
       <c r="N23" s="14"/>
     </row>
-    <row r="24" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="32"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -1627,7 +1627,7 @@
       <c r="M24" s="21"/>
       <c r="N24" s="14"/>
     </row>
-    <row r="25" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="25" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="33"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -1636,22 +1636,22 @@
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
       <c r="I25" s="14"/>
-      <c r="K25" s="34" t="s">
-        <v>13</v>
+      <c r="K25" s="30" t="s">
+        <v>12</v>
       </c>
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
       <c r="N25" s="14"/>
     </row>
-    <row r="26" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A26" s="34" t="s">
-        <v>20</v>
+    <row r="26" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="30" t="s">
+        <v>19</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="14"/>
-      <c r="F26" s="34" t="s">
-        <v>14</v>
+      <c r="F26" s="30" t="s">
+        <v>13</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
@@ -1661,7 +1661,7 @@
       <c r="M26" s="20"/>
       <c r="N26" s="14"/>
     </row>
-    <row r="27" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="32"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -1675,7 +1675,7 @@
       <c r="M27" s="20"/>
       <c r="N27" s="14"/>
     </row>
-    <row r="28" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="28" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="32"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -1689,26 +1689,26 @@
       <c r="M28" s="21"/>
       <c r="N28" s="14"/>
     </row>
-    <row r="29" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="29" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="32"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="14"/>
-      <c r="F29" s="34" t="s">
-        <v>18</v>
+      <c r="F29" s="30" t="s">
+        <v>17</v>
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
       <c r="I29" s="14"/>
-      <c r="K29" s="34" t="s">
-        <v>17</v>
+      <c r="K29" s="30" t="s">
+        <v>16</v>
       </c>
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
       <c r="N29" s="14"/>
     </row>
-    <row r="30" spans="1:14" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A30" s="35"/>
+    <row r="30" spans="1:14" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="31"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="18"/>
@@ -1721,8 +1721,8 @@
       <c r="M30" s="20"/>
       <c r="N30" s="14"/>
     </row>
-    <row r="31" spans="1:14" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="F31" s="35"/>
+    <row r="31" spans="1:14" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="F31" s="31"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="8"/>
@@ -1731,57 +1731,50 @@
       <c r="M31" s="21"/>
       <c r="N31" s="14"/>
     </row>
-    <row r="32" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="K32" s="34" t="s">
-        <v>24</v>
+    <row r="32" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K32" s="30" t="s">
+        <v>23</v>
       </c>
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
       <c r="N32" s="14"/>
     </row>
-    <row r="33" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="33" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K33" s="32"/>
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
       <c r="N33" s="14"/>
     </row>
-    <row r="34" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="34" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K34" s="32"/>
       <c r="L34" s="20"/>
       <c r="M34" s="20"/>
       <c r="N34" s="14"/>
     </row>
-    <row r="35" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="35" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K35" s="33"/>
       <c r="L35" s="21"/>
       <c r="M35" s="21"/>
       <c r="N35" s="14"/>
     </row>
-    <row r="36" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="K36" s="34" t="s">
-        <v>21</v>
+    <row r="36" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K36" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="L36" s="20"/>
       <c r="M36" s="20"/>
       <c r="N36" s="14"/>
     </row>
-    <row r="37" spans="11:14" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="K37" s="35"/>
+    <row r="37" spans="11:14" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="K37" s="31"/>
       <c r="L37" s="22"/>
       <c r="M37" s="22"/>
       <c r="N37" s="23"/>
     </row>
-    <row r="38" spans="11:14" ht="73.5" customHeight="1" x14ac:dyDescent="0.65"/>
-    <row r="39" spans="11:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.65"/>
+    <row r="38" spans="11:14" ht="73.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="39" spans="11:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="K29:K31"/>
-    <mergeCell ref="K32:K35"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="K11:M11"/>
@@ -1792,6 +1785,13 @@
     <mergeCell ref="F20:F25"/>
     <mergeCell ref="K20:K24"/>
     <mergeCell ref="A21:A25"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="K29:K31"/>
+    <mergeCell ref="K32:K35"/>
   </mergeCells>
   <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.3" footer="0.3"/>
   <pageSetup scale="40" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed Module 2 assignment
</commit_message>
<xml_diff>
--- a/Module2/Assignment/Worksheet 2 - Immune Cell Type.xlsx
+++ b/Module2/Assignment/Worksheet 2 - Immune Cell Type.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvesgreatti/github/Immunoengineering/Module2/Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1626D0AC-E8F7-344E-BB57-64BA755CD5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD11135-F569-8745-B815-ED3DE0DB5513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3060" yWindow="9060" windowWidth="38900" windowHeight="13340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cell summary sheet blank" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="149">
   <si>
     <t>Immune Cell</t>
   </si>
@@ -232,9 +232,6 @@
     <t>Promotes antibody production</t>
   </si>
   <si>
-    <t>Support B cell division and maturation</t>
-  </si>
-  <si>
     <t>Bridge between innate and adaptive immne responses</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
   </si>
   <si>
     <t>government</t>
-  </si>
-  <si>
-    <t>co-stimulatory signals</t>
   </si>
   <si>
     <t>DCS provide co-stimulatory signals through the interaction of surface molecules such as CD80/CD86 (on DCs) with CD28 (on T cells)</t>
@@ -350,9 +344,6 @@
     <t>Follicular DCs capture opsonized antigens and display these antigens to B cells to be activated. The follicle become a center of B cell proliferation.</t>
   </si>
   <si>
-    <t>FDCs release factord, such as profiferation-inducing ligand (APRIL) or B-cell activating factor (BAFF) which co-stimulate B cells.</t>
-  </si>
-  <si>
     <t>B cell activation</t>
   </si>
   <si>
@@ -365,9 +356,6 @@
     <t>Acts a barrier</t>
   </si>
   <si>
-    <t>The skin has tigth epithelial cells which protect naturally against external pathoegems and if they enter the body , a sticky mucus captures them and cleams them out</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reduces UV radiation </t>
   </si>
   <si>
@@ -386,9 +374,6 @@
     <t>Skin particiopates in thermal regulation by conserving or releasing heat</t>
   </si>
   <si>
-    <t xml:space="preserve">The skin maintains the body's water and homeostatic balance (tight cell junctions, sebaceous glands, sweat glands, moisturinzing factors) </t>
-  </si>
-  <si>
     <t>Keratinocytes, the predominant cells in the epidermis; express Tool-like receptors (TLRs) which are pattern-recognition receptors (PRRs) triggering an infrlammatory response</t>
   </si>
   <si>
@@ -398,9 +383,6 @@
     <t>Certain complement proteins , such as C3a and C5b stimulate the recruitment of immune cells like macrophages</t>
   </si>
   <si>
-    <t>membrane attack complex</t>
-  </si>
-  <si>
     <t>Chemoattractants</t>
   </si>
   <si>
@@ -410,9 +392,6 @@
     <t>Enhancement of adaptive immune system</t>
   </si>
   <si>
-    <t>Complement activation can increase antibody-dependent cellular cytoxicity (ADCC) and complement dependent cytoxicity (DCC)</t>
-  </si>
-  <si>
     <t>Clearance of immune complexes</t>
   </si>
   <si>
@@ -422,26 +401,9 @@
     <t>Stimulation of B cells</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Complement </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>activaition via CR1/2/CD19/TAPA-1 can participate to the costimulation of B cells enhancing clonal expansion and germinal center formation</t>
-    </r>
-  </si>
-  <si>
     <t>Recognition of class of invaders</t>
   </si>
   <si>
-    <t>TLRs are pattern-recognition recptors designed tp recognize microbial attacks; among them TLR4 is used by macropages to sense the presence of lipopolysaccharide (LPS); TL7 detects single-stranded RNA of viruses whereas TLR9 recognized double-stranded DNA of bacteria and simple viruses</t>
-  </si>
-  <si>
     <t>Activation of immune responses</t>
   </si>
   <si>
@@ -451,18 +413,12 @@
     <t>Cytokine production</t>
   </si>
   <si>
-    <t>TLR signaling can induce the productionof cytokines such as IL-12 and TNF-alpha in DCs; recruiting immune cells to the site of  infection and activate them</t>
-  </si>
-  <si>
     <t>Enhanced antige-presentation</t>
   </si>
   <si>
     <t>The recognition of invading microbes by TLRS enhance antigen presentation to naïve T cells.</t>
   </si>
   <si>
-    <t>neutralisation</t>
-  </si>
-  <si>
     <t>Antibody-dependent cellular cytotoxicity (ADCC)</t>
   </si>
   <si>
@@ -472,18 +428,9 @@
     <t>Acts as a sensory organ</t>
   </si>
   <si>
-    <t>Antibodies recognize specific antigens (IgG antibodies). The Fc regionof the bound antibodies interact with Fc receptors on the surface of the NK cells. This activation primes the NL cells for cytotoxic activity.</t>
-  </si>
-  <si>
     <t>IgM antibodies can neutralize viruses by binding to them preventing them from infecting cells.</t>
   </si>
   <si>
-    <t>Complement mediated can cause the lysis of bacterial cells through the formation of a menbrane Attack Complex (MAC) which makes holes in the targeted cells, causing its deaths</t>
-  </si>
-  <si>
-    <t>filtering of foreign substances and pathogens: T and B cells, and antigen-presenting cells (APCs) are present within lymph nodes to detect anitgens</t>
-  </si>
-  <si>
     <t>Immune monitoring</t>
   </si>
   <si>
@@ -514,15 +461,9 @@
     <t>Transport of immune cells</t>
   </si>
   <si>
-    <t>Dendrictic ells leave the tissues and travel through the lymphatic system to the nearest lymph node to activate naïve T cells. Lemphatic vessesl transport immune cells and APCs between lymph nodes and tissues.</t>
-  </si>
-  <si>
     <t>Anigen processing</t>
   </si>
   <si>
-    <t>Once DCs have captured antigens, they break them down into smaller fragments, exposing many facettes of the antigens. The fragments are them presented to T cells with MCh molecules.</t>
-  </si>
-  <si>
     <t>They produce different cytokines, chemokines, and other substances to recruit other immune cells, and promote inflammatory process.</t>
   </si>
   <si>
@@ -530,13 +471,58 @@
   </si>
   <si>
     <t>Neutrophils can phagocytose and clear cellular debris, including dead cells.</t>
+  </si>
+  <si>
+    <t>TLRs are pattern-recognition receptors designed to recognize microbial attacks; among them TLR4 is used by macropages to sense the presence of lipopolysaccharide (LPS); TLR7 detects single-stranded RNA of viruses whereas TLR9 recognized double-stranded DNA of bacteria and simple viruses</t>
+  </si>
+  <si>
+    <t>Once DCs have captured antigens, they break them down into smaller fragments, exposing many facettes of the antigens. The fragments are them presented to T cells with MCH molecules.</t>
+  </si>
+  <si>
+    <t>FDCs release factors, such as profiferation-inducing ligand (APRIL) or B-cell activating factor (BAFF) which co-stimulate B cells.</t>
+  </si>
+  <si>
+    <t>The skin has tigth epithelial cells which protect naturally against external pathogens and if they enter the body , a sticky mucus captures them and clears them out</t>
+  </si>
+  <si>
+    <t>Co-stimulatory signals</t>
+  </si>
+  <si>
+    <t>Membrane attack complex</t>
+  </si>
+  <si>
+    <t>Neutralisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The skin maintains the body's water and homeostatic balance (using tight cell junctions, sebaceous glands, sweat glands, moisturinzing factors) </t>
+  </si>
+  <si>
+    <t>Complement activation can increase antibody-dependent cellular cytotoxicity (ADCC) and complement dependent cytotoxicity (DCC)</t>
+  </si>
+  <si>
+    <t>Complement activation via CR1/2/CD19/TAPA-1 can participate to the costimulation of B cells enhancing clonal expansion and germinal center formation</t>
+  </si>
+  <si>
+    <t>TLR signaling can induce the production of cytokines such as IL-12 and TNF-alpha in DCs; recruiting immune cells to the site of  infection and activate them</t>
+  </si>
+  <si>
+    <t>Antibodies recognize specific antigens (IgG antibodies). The Fc region of the bound antibodies interact with Fc receptors on the surface of the NK cells. This activation primes the NL cells for cytotoxic activity.</t>
+  </si>
+  <si>
+    <t>Complement mediated can cause the lysis of bacterial cells through the formation of a menbrane attack Complex (MAC) which makes holes in the targeted cell, causing its deaths.</t>
+  </si>
+  <si>
+    <t>Filtering of foreign substances and pathogens: T and B cells, and antigen-presenting cells (APCs) are present within lymph nodes to detect antigens</t>
+  </si>
+  <si>
+    <t>Dendrictic cells leave the tissues and travel through the lymphatic system to the nearest lymph node to activate naïve T cells. Lymphatic vessels transport immune cells and APCs between lymph nodes and tissues.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,12 +572,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -601,7 +581,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -670,17 +650,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -694,17 +663,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -732,11 +690,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -748,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -766,9 +726,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -778,10 +735,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -793,49 +750,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -843,11 +767,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -855,46 +785,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1752,8 +1664,8 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14:N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1761,74 +1673,74 @@
     <col min="1" max="1" width="21.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="70.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23" style="1" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" customWidth="1"/>
-    <col min="14" max="14" width="85.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="87" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="35" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="20" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="20" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="20" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="23" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="32" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+    <row r="11" spans="1:14" ht="25" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="38" t="s">
+      <c r="F11" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
       <c r="I11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="38" t="s">
+      <c r="K11" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
       <c r="N11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1873,572 +1785,565 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="25" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="39" t="s">
+      <c r="F14" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G14" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="39" t="s">
+      <c r="K14" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="16"/>
-      <c r="M14" s="44" t="s">
+      <c r="L14" s="15"/>
+      <c r="M14" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="N14" s="30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="71.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="26"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="26"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="26"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="N15" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="26"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="27"/>
+      <c r="G16" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="K16" s="26"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="N16" s="30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="26"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="K17" s="26"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="N17" s="30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="26"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="26"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="K18" s="26"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="N14" s="45" t="s">
+      <c r="N18" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="26"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="27"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="I19" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="K19" s="27"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="30" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="71.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="40"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="K15" s="40"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="46" t="s">
+      <c r="N19" s="30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="27"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" s="16"/>
+      <c r="M20" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="N20" s="30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="26"/>
+      <c r="G21" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="K21" s="26"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="N21" s="30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="26"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="26"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="I22" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="K22" s="26"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="N22" s="30" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="26"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="26"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="K23" s="26"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="N23" s="30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="26"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="26"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="K24" s="27"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="N24" s="30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="27"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="27"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="I25" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="K25" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="16"/>
+      <c r="M25" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="N25" s="34" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="16"/>
+      <c r="H26" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="K26" s="26"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="N26" s="30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="26"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="26"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="K27" s="26"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="N27" s="30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="26"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="27"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="I28" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="K28" s="27"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="N28" s="30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="26"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="16"/>
+      <c r="H29" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="K29" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="L29" s="16"/>
+      <c r="M29" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="N29" s="30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="25"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="26"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="K30" s="26"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="N30" s="30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="F31" s="25"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="I31" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K31" s="27"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="N31" s="30" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K32" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="L32" s="16"/>
+      <c r="M32" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="N32" s="30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K33" s="26"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="N33" s="30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K34" s="26"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="N34" s="30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K35" s="27"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="N35" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K36" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" s="16"/>
+      <c r="M36" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="N36" s="30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="11:14" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="K37" s="25"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="N15" s="50" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="40"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="K16" s="40"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="N16" s="50" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="40"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="H17" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="K17" s="40"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="N17" s="50" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="40"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="I18" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="K18" s="40"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="N18" s="50" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="40"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="41"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="49" t="s">
+      <c r="N37" s="37" t="s">
         <v>148</v>
-      </c>
-      <c r="I19" s="50" t="s">
-        <v>149</v>
-      </c>
-      <c r="K19" s="41"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="N19" s="50" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="41"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="K20" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="L20" s="17"/>
-      <c r="M20" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="N20" s="50" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="40"/>
-      <c r="G21" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="K21" s="40"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="N21" s="50" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="40"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="40"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="I22" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="K22" s="40"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="46" t="s">
-        <v>112</v>
-      </c>
-      <c r="N22" s="50" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="40"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="40"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K23" s="40"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="N23" s="50" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="40"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="40"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="I24" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="K24" s="41"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="N24" s="50" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="41"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="41"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="I25" s="50" t="s">
-        <v>146</v>
-      </c>
-      <c r="K25" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="L25" s="17"/>
-      <c r="M25" s="46" t="s">
-        <v>118</v>
-      </c>
-      <c r="N25" s="47" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="F26" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="I26" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="K26" s="40"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="N26" s="50" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="40"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" s="40"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="I27" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="K27" s="40"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="N27" s="50" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="40"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="F28" s="41"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="I28" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="K28" s="41"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="N28" s="50" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="40"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="F29" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="I29" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="K29" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="L29" s="17"/>
-      <c r="M29" s="46" t="s">
-        <v>126</v>
-      </c>
-      <c r="N29" s="50" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="43"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="F30" s="40"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="I30" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="K30" s="40"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="46" t="s">
-        <v>127</v>
-      </c>
-      <c r="N30" s="50" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F31" s="43"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="K31" s="41"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="49" t="s">
-        <v>128</v>
-      </c>
-      <c r="N31" s="50" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K32" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="L32" s="17"/>
-      <c r="M32" s="51" t="s">
-        <v>134</v>
-      </c>
-      <c r="N32" s="46" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K33" s="40"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="46" t="s">
-        <v>136</v>
-      </c>
-      <c r="N33" s="50" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K34" s="40"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="N34" s="50" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K35" s="41"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="49" t="s">
-        <v>139</v>
-      </c>
-      <c r="N35" s="50" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36" spans="11:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K36" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="L36" s="17"/>
-      <c r="M36" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="N36" s="50" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="11:14" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="K37" s="43"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="52" t="s">
-        <v>143</v>
-      </c>
-      <c r="N37" s="53" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="38" spans="11:14" ht="73.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="39" spans="11:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="K29:K31"/>
-    <mergeCell ref="K32:K35"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="K11:M11"/>
@@ -2449,6 +2354,13 @@
     <mergeCell ref="F20:F25"/>
     <mergeCell ref="K20:K24"/>
     <mergeCell ref="A21:A25"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="K29:K31"/>
+    <mergeCell ref="K32:K35"/>
   </mergeCells>
   <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.3" footer="0.3"/>
   <pageSetup scale="40" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>